<commit_message>
build RAD.IRA 1.0.0 trial-implementation
</commit_message>
<xml_diff>
--- a/RAD/IRA/observations-summary.xlsx
+++ b/RAD/IRA/observations-summary.xlsx
@@ -166,10 +166,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyBorder="true" applyFill="true" applyFont="true">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true" applyFont="true">
       <alignment vertical="top" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment vertical="top" wrapText="true"/>
     </xf>
   </cellXfs>

</xml_diff>